<commit_message>
Updated logbook and added Sprint 1 Presentation
</commit_message>
<xml_diff>
--- a/Yousif/Efforts Logbook.xlsx
+++ b/Yousif/Efforts Logbook.xlsx
@@ -5,21 +5,26 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yousif/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yousif/Oasis/GitHub/CSI-4999/Yousif/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B14BF9B-94FD-1049-8E5C-569DB57146C3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D07429-E54A-254A-BAEE-93EE845344D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2540" yWindow="6480" windowWidth="21240" windowHeight="14720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Evidence" sheetId="1" r:id="rId1"/>
     <sheet name="Count" sheetId="25" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -29,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Brief Description of Acomplishments</t>
   </si>
@@ -37,9 +42,6 @@
     <t>Wrote usecases UC1, UC2. Developed practice and proceedure for effectively using GIT</t>
   </si>
   <si>
-    <t>You must provide accurate artifacts created by you. For example</t>
-  </si>
-  <si>
     <t>Artifact Name</t>
   </si>
   <si>
@@ -131,6 +133,22 @@
   </si>
   <si>
     <t>1 (Tools, Technology, and Algorithm Development), 6[CS] (Algorithms Design and Development)</t>
+  </si>
+  <si>
+    <t>Made decisions on which python libraries are needed and will be used for the backend AI/ML implementation of the project.
+Algorithm extension of ability to alter the algorithm using BeautifulSoup (web scrapper) to scrap the news and look for keywords on particular stocks and their related companies.</t>
+  </si>
+  <si>
+    <t>Sprint 1 Presentation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You must provide accurate artifacts created by you. </t>
+  </si>
+  <si>
+    <t>Sprint 1 Presentation.pptx</t>
+  </si>
+  <si>
+    <t>Slides 3-7</t>
   </si>
 </sst>
 </file>
@@ -291,9 +309,6 @@
   <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -318,23 +333,23 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -348,49 +363,52 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -675,119 +693,129 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="23" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="23" customWidth="1"/>
-    <col min="4" max="4" width="27.5" style="23" customWidth="1"/>
-    <col min="5" max="5" width="42.5" style="23" customWidth="1"/>
-    <col min="6" max="6" width="15.5" style="23" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="23" customWidth="1"/>
-    <col min="8" max="8" width="28" style="23" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="23"/>
+    <col min="1" max="1" width="8.6640625" style="22" customWidth="1"/>
+    <col min="2" max="2" width="17.5" style="22" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="22" customWidth="1"/>
+    <col min="4" max="4" width="27.5" style="22" customWidth="1"/>
+    <col min="5" max="5" width="42.5" style="22" customWidth="1"/>
+    <col min="6" max="6" width="15.5" style="22" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="22" customWidth="1"/>
+    <col min="8" max="8" width="28" style="22" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+    <row r="1" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+    </row>
+    <row r="2" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="13"/>
+      <c r="C2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-    </row>
-    <row r="2" spans="1:8" ht="41" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="25"/>
-      <c r="C2" s="24" t="s">
+      <c r="D2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+    </row>
+    <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="27"/>
+      <c r="C3" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="31">
+        <v>16</v>
+      </c>
+      <c r="D4" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="32" t="s">
+        <v>5</v>
+      </c>
+      <c r="G4" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="119" x14ac:dyDescent="0.2">
+      <c r="A5" s="30" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="30"/>
+      <c r="C5" s="33">
+        <v>10</v>
+      </c>
+      <c r="D5" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="17"/>
-    </row>
-    <row r="3" spans="1:8" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="28"/>
-      <c r="C3" s="29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="29" t="s">
-        <v>11</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="G3" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="29" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="32">
-        <v>16</v>
-      </c>
-      <c r="D4" s="32" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A5" s="31" t="s">
+      <c r="E5" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="34" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="31"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33" t="s">
-        <v>33</v>
-      </c>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="31"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="33"/>
       <c r="D6" s="33"/>
       <c r="E6" s="34"/>
@@ -796,10 +824,10 @@
       <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="31"/>
+      <c r="A7" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="30"/>
       <c r="C7" s="33"/>
       <c r="D7" s="33"/>
       <c r="E7" s="34"/>
@@ -809,7 +837,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B8" s="36"/>
       <c r="C8" s="33"/>
@@ -821,7 +849,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="35" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B9" s="36"/>
       <c r="C9" s="33"/>
@@ -833,7 +861,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B10" s="36"/>
       <c r="C10" s="33"/>
@@ -845,7 +873,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="36"/>
       <c r="C11" s="33"/>
@@ -857,7 +885,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="36"/>
       <c r="C12" s="33"/>
@@ -869,21 +897,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:H1"/>
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -907,209 +935,209 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="34" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="20"/>
+      <c r="C1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="20" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
     </row>
     <row r="2" spans="1:9" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="14"/>
+      <c r="A2" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="15"/>
+      <c r="C2" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="15"/>
     </row>
     <row r="3" spans="1:9" ht="22" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="18"/>
+      <c r="I3" s="18"/>
     </row>
     <row r="4" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6">
+        <v>1</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2</v>
+      </c>
+      <c r="E4" s="6">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6">
+        <v>4</v>
+      </c>
+      <c r="G4" s="6">
+        <v>5</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C5" s="8">
+        <v>2</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="10">
         <v>1</v>
       </c>
-      <c r="D4" s="7">
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>5</v>
+      </c>
+      <c r="H5" s="8">
         <v>2</v>
       </c>
-      <c r="E4" s="7">
+      <c r="I5" s="8">
         <v>3</v>
       </c>
-      <c r="F4" s="7">
+    </row>
+    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7">
+        <v>3</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="7">
         <v>4</v>
       </c>
-      <c r="G4" s="7">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="7">
         <v>5</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" s="4" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="9">
-        <v>0</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="9">
-        <v>2</v>
-      </c>
-      <c r="D5" s="9">
-        <v>3</v>
-      </c>
-      <c r="E5" s="11">
-        <v>1</v>
-      </c>
-      <c r="F5" s="9">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
-        <v>5</v>
-      </c>
-      <c r="H5" s="9">
-        <v>2</v>
-      </c>
-      <c r="I5" s="9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8">
-        <v>1</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8">
-        <v>2</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="8">
-        <v>3</v>
-      </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="8">
-        <v>4</v>
-      </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="8">
-        <v>5</v>
-      </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
     </row>
     <row r="11" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>6</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="8">
+      <c r="A12" s="7">
         <v>7</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>8</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>